<commit_message>
Applied Guen-Guec rule part2
</commit_message>
<xml_diff>
--- a/src/data/CalculateSakawiAwal.xlsx
+++ b/src/data/CalculateSakawiAwal.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT PROJECTS\SakawiCham\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT PROJECTS\sakawi-cham-web\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="getAwalDateByGregoryDate()" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t xml:space="preserve">Lieh </t>
   </si>
@@ -87,6 +88,39 @@
   </si>
   <si>
     <t>const result = n - (m * Math.floor(n / m));</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>Thu 2</t>
+  </si>
+  <si>
+    <t>Thu 3</t>
+  </si>
+  <si>
+    <t>Thu 4</t>
+  </si>
+  <si>
+    <t>Thu 5</t>
+  </si>
+  <si>
+    <t>Thu 6</t>
+  </si>
+  <si>
+    <t>Thu 7</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>x &gt; y</t>
+  </si>
+  <si>
+    <t>y + (6-x) + 1</t>
   </si>
 </sst>
 </file>
@@ -456,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,4 +923,95 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="4.42578125" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>